<commit_message>
Updated Core classes from other branch
</commit_message>
<xml_diff>
--- a/WebServiceTests/Resources/TestSuite.xlsx
+++ b/WebServiceTests/Resources/TestSuite.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>

</xml_diff>